<commit_message>
added logic and tested to parse across panes in xlsx
</commit_message>
<xml_diff>
--- a/backend/scraper/municipalities.xlsx
+++ b/backend/scraper/municipalities.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaceSpeak\newsfeed\backend\scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4157937B-7414-4989-B8B0-1B3E5247471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643F2876-5CF3-4994-BD9E-A7B255C1EB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{D43231DE-8247-43E5-8A59-41D1B75030BB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D43231DE-8247-43E5-8A59-41D1B75030BB}"/>
   </bookViews>
   <sheets>
     <sheet name="British Columbia" sheetId="1" r:id="rId1"/>
+    <sheet name="Alberta" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -44,9 +45,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Regional District</t>
-  </si>
-  <si>
     <t>Vancouver</t>
   </si>
   <si>
@@ -62,31 +60,25 @@
     <t>City</t>
   </si>
   <si>
-    <t>Metro Vancouver</t>
-  </si>
-  <si>
-    <t>Central Okanagan</t>
-  </si>
-  <si>
-    <t>Thompson-Nicola</t>
-  </si>
-  <si>
     <t>Saanich</t>
   </si>
   <si>
     <t>District municipality</t>
   </si>
   <si>
-    <t>Capital</t>
-  </si>
-  <si>
     <t>Surrey</t>
   </si>
   <si>
     <t>Abbotsford</t>
   </si>
   <si>
-    <t>Fraser Valley</t>
+    <t>Banff</t>
+  </si>
+  <si>
+    <t>Town</t>
+  </si>
+  <si>
+    <t>Camrose</t>
   </si>
 </sst>
 </file>
@@ -469,100 +461,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7AF1A5-674B-4BFA-B978-6EEC553F95E7}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -577,4 +545,62 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F589343-CE6D-4228-A109-1BF674F546C0}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="A4:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6C02A791-2E86-42E5-9B13-63A8FAACB07C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{97E2B566-E1D8-41DA-88B4-CDF04F59888A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>